<commit_message>
Test Cases: Discount code
</commit_message>
<xml_diff>
--- a/testStrategy/test_cases_new_feature_discount_code.xlsx
+++ b/testStrategy/test_cases_new_feature_discount_code.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -50,6 +50,57 @@
   </si>
   <si>
     <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Booking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valid Discount code – user can proceed with payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is on passenger details page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter a valid email, first and last name.
+2. Fill other required fields correctly.
+3. Get a correct discount code and set it to the Discount code field
+4. Click continue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System allows user to proceed with payment and applies all data including discount code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive / Validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To_Be_Automated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discount code field is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter a valid email, first and last name.
+2. Fill other required fields correctly.
+3. Leave Discount code field empty
+4. Click continue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System displays a validation error indicating the discount code is invalid and does not proceed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative / Validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid discount code value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter a valid email, first and last name.
+2. Fill other required fields correctly.
+3. Set an invalid discount code
+4. Click continue.</t>
   </si>
 </sst>
 </file>
@@ -59,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +140,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -146,7 +203,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -169,6 +226,14 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -426,7 +491,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -474,14 +539,92 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G4" s="2"/>
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="2"/>

</xml_diff>